<commit_message>
Update the first test case and add a new one
</commit_message>
<xml_diff>
--- a/test/Test cases.xlsx
+++ b/test/Test cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\maze-project-2021\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8089C97E-E81D-4F35-B3EC-586A442B5F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0B57D9-4A73-439A-8EBE-CEDDBAE98932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27210" windowHeight="15990" activeTab="1" xr2:uid="{D88C0871-9CFF-47EC-A37B-1CA9AB3CB744}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
@@ -77,6 +77,37 @@
   </si>
   <si>
     <t>Passed</t>
+  </si>
+  <si>
+    <t>The test has
+been done manually</t>
+  </si>
+  <si>
+    <t>1. The algorithm takes 
+ the given parameters</t>
+  </si>
+  <si>
+    <t>2. The maze is printed
+ properly</t>
+  </si>
+  <si>
+    <t>Function 
+getWidth</t>
+  </si>
+  <si>
+    <t>1.Input width</t>
+  </si>
+  <si>
+    <t>2.Check if the function 
+takes the input</t>
+  </si>
+  <si>
+    <t>The function takes the 
+given input</t>
+  </si>
+  <si>
+    <t>The function receives 
+and takes the input</t>
   </si>
 </sst>
 </file>
@@ -101,7 +132,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,8 +145,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -167,17 +204,6 @@
       <right style="thick">
         <color indexed="64"/>
       </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thick">
         <color indexed="64"/>
@@ -243,6 +269,32 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top style="thick">
+        <color theme="1"/>
+      </top>
+      <bottom style="thick">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="1"/>
+      </right>
+      <top style="thick">
+        <color theme="1"/>
+      </top>
+      <bottom style="thick">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="1"/>
+      </left>
       <right style="thick">
         <color theme="1"/>
       </right>
@@ -251,77 +303,22 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color theme="1"/>
-      </top>
-      <bottom style="thick">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <left style="thick">
+        <color theme="1"/>
+      </left>
       <right style="thick">
         <color theme="1"/>
       </right>
       <top style="thick">
         <color theme="1"/>
       </top>
-      <bottom style="thick">
-        <color theme="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thick">
         <color theme="1"/>
       </left>
-      <right style="thick">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="1"/>
-      </left>
-      <right style="thick">
-        <color theme="1"/>
-      </right>
-      <top style="thick">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="1"/>
-      </left>
-      <right style="thick">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thick">
         <color theme="1"/>
       </right>
@@ -335,16 +332,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -360,52 +353,77 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -729,7 +747,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,188 +762,195 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23">
+    <row r="2" spans="1:10" ht="80.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="7" t="s">
+      <c r="F2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="20"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="3"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="26"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="E2:E3"/>
+    <mergeCell ref="G2:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -937,7 +962,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,142 +977,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27">
+      <c r="A2" s="23">
         <v>2</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="16"/>
+      <c r="B2" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="16"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="16"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="32"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="31"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D13" s="9"/>
+      <c r="D13" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="8">
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="G2:G5"/>
     <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D2:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add a third test case
</commit_message>
<xml_diff>
--- a/test/Test cases.xlsx
+++ b/test/Test cases.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\maze-project-2021\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0B57D9-4A73-439A-8EBE-CEDDBAE98932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D925E79-D471-46AF-8A35-0744F1A9CFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27210" windowHeight="15990" activeTab="1" xr2:uid="{D88C0871-9CFF-47EC-A37B-1CA9AB3CB744}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27210" windowHeight="15990" activeTab="2" xr2:uid="{D88C0871-9CFF-47EC-A37B-1CA9AB3CB744}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -91,10 +92,6 @@
  properly</t>
   </si>
   <si>
-    <t>Function 
-getWidth</t>
-  </si>
-  <si>
     <t>1.Input width</t>
   </si>
   <si>
@@ -108,6 +105,14 @@
   <si>
     <t>The function receives 
 and takes the input</t>
+  </si>
+  <si>
+    <t>Function 
+getWidth in checkedMaze</t>
+  </si>
+  <si>
+    <t>Function 
+getWidth in maze</t>
   </si>
 </sst>
 </file>
@@ -152,7 +157,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -328,11 +333,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -374,6 +423,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -392,38 +444,56 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -785,10 +855,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="80.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -797,30 +867,30 @@
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="22" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="24" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20"/>
-      <c r="B3" s="18"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="22"/>
+      <c r="E3" s="23"/>
       <c r="F3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="26"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
@@ -961,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70FB507A-0229-41BF-818F-AEC3B7FF2E89}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,56 +1070,56 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23">
+      <c r="A2" s="32">
         <v>2</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="D2" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
@@ -1107,7 +1177,7 @@
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="33"/>
+      <c r="F11" s="17"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
@@ -1138,4 +1208,114 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EACF856B-6ABF-4C89-B87E-55B3E48903E1}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="37">
+        <v>3</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="38"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="38"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="35"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="39"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add a fourth test case
</commit_message>
<xml_diff>
--- a/test/Test cases.xlsx
+++ b/test/Test cases.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\maze-project-2021\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D925E79-D471-46AF-8A35-0744F1A9CFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9FCD8F-A87E-4913-9E8E-015C454E853E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27210" windowHeight="15990" activeTab="2" xr2:uid="{D88C0871-9CFF-47EC-A37B-1CA9AB3CB744}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27210" windowHeight="15990" activeTab="3" xr2:uid="{D88C0871-9CFF-47EC-A37B-1CA9AB3CB744}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="Лист4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -113,6 +114,13 @@
   <si>
     <t>Function 
 getWidth in maze</t>
+  </si>
+  <si>
+    <t>Function 
+getHeight in checkedMaze</t>
+  </si>
+  <si>
+    <t>1.Input height</t>
   </si>
 </sst>
 </file>
@@ -426,6 +434,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -474,7 +485,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -490,9 +501,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -855,10 +863,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="80.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -867,30 +875,30 @@
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="25" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="23"/>
+      <c r="E3" s="24"/>
       <c r="F3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="25"/>
+      <c r="G3" s="26"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
@@ -1032,7 +1040,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G5"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,56 +1078,56 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32">
+      <c r="A2" s="33">
         <v>2</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="30" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="33" t="s">
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
@@ -1214,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EACF856B-6ABF-4C89-B87E-55B3E48903E1}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,7 +1246,7 @@
       <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
@@ -1247,73 +1255,183 @@
       <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37">
+      <c r="A2" s="38">
         <v>3</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36" t="s">
+      <c r="A4" s="39"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="F2:F5"/>
     <mergeCell ref="G2:G5"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="B2:B5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9E0783-F8BC-47CA-9BBC-F36BBA6BD7EA}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
+        <v>4</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="36"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="G2:G5"/>
     <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="E2:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update previous test cases and add a fifth
</commit_message>
<xml_diff>
--- a/test/Test cases.xlsx
+++ b/test/Test cases.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\maze-project-2021\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9FCD8F-A87E-4913-9E8E-015C454E853E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA3DD16-924F-49E4-8236-1947805643A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27210" windowHeight="15990" activeTab="3" xr2:uid="{D88C0871-9CFF-47EC-A37B-1CA9AB3CB744}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27210" windowHeight="15990" activeTab="4" xr2:uid="{D88C0871-9CFF-47EC-A37B-1CA9AB3CB744}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
     <sheet name="Лист4" sheetId="4" r:id="rId4"/>
+    <sheet name="Лист5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -121,6 +122,10 @@
   </si>
   <si>
     <t>1.Input height</t>
+  </si>
+  <si>
+    <t>Function 
+getHeight in maze</t>
   </si>
 </sst>
 </file>
@@ -485,7 +490,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -494,13 +505,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1120,7 +1125,7 @@
       <c r="F4" s="31"/>
       <c r="G4" s="31"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="32"/>
       <c r="B5" s="32"/>
       <c r="C5" s="32"/>
@@ -1260,7 +1265,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38">
+      <c r="A2" s="35">
         <v>3</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -1283,27 +1288,27 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37" t="s">
+      <c r="A4" s="36"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+    </row>
+    <row r="5" spans="1:7" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="37"/>
       <c r="B5" s="20"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
@@ -1314,14 +1319,14 @@
     <row r="6" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="B2:B5"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="F2:F5"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="B2:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1332,8 +1337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9E0783-F8BC-47CA-9BBC-F36BBA6BD7EA}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,26 +1398,26 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37" t="s">
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="38"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+    </row>
+    <row r="5" spans="1:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22"/>
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
@@ -1436,4 +1441,117 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B300D546-F4BD-437E-B626-2A42F83D89FB}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
+        <v>5</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="38"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+    </row>
+    <row r="5" spans="1:7" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="E2:E5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add a seventh testcase
</commit_message>
<xml_diff>
--- a/test/Test cases.xlsx
+++ b/test/Test cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\maze-project-2021\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA3DD16-924F-49E4-8236-1947805643A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6961E56-CD71-4CC4-8477-6734698380DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27210" windowHeight="15990" activeTab="4" xr2:uid="{D88C0871-9CFF-47EC-A37B-1CA9AB3CB744}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27210" windowHeight="15990" activeTab="5" xr2:uid="{D88C0871-9CFF-47EC-A37B-1CA9AB3CB744}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
     <sheet name="Лист4" sheetId="4" r:id="rId4"/>
     <sheet name="Лист5" sheetId="5" r:id="rId5"/>
+    <sheet name="Лист6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -126,6 +127,28 @@
   <si>
     <t>Function 
 getHeight in maze</t>
+  </si>
+  <si>
+    <t>Function 
+isInBound in maze</t>
+  </si>
+  <si>
+    <t>1.Check if the function takes the inputed width and height</t>
+  </si>
+  <si>
+    <t>2.Check the weather the "if" condition statements in the function work</t>
+  </si>
+  <si>
+    <t>1.The function takes the with and height</t>
+  </si>
+  <si>
+    <t>2. The "if" condition statements work and a result is received</t>
+  </si>
+  <si>
+    <t>1.The function successfully takes the with and height</t>
+  </si>
+  <si>
+    <t>2.The "if" condition statements works and a the function returns "true" or "false"</t>
   </si>
 </sst>
 </file>
@@ -490,20 +513,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1265,7 +1288,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35">
+      <c r="A2" s="37">
         <v>3</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -1288,27 +1311,27 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
       <c r="E3" s="40"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39" t="s">
+      <c r="A4" s="38"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="35"/>
       <c r="E4" s="40"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
     </row>
     <row r="5" spans="1:7" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="20"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
@@ -1398,24 +1421,24 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
       <c r="E3" s="40"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="39" t="s">
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="35"/>
       <c r="E4" s="40"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
     </row>
     <row r="5" spans="1:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22"/>
@@ -1447,8 +1470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B300D546-F4BD-437E-B626-2A42F83D89FB}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1508,24 +1531,24 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
       <c r="E3" s="40"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="39" t="s">
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="35"/>
       <c r="E4" s="40"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
     </row>
     <row r="5" spans="1:7" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22"/>
@@ -1554,4 +1577,120 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDD3808-7269-4705-8859-387567E01703}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="51" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
+        <v>6</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="35"/>
+    </row>
+    <row r="4" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="40"/>
+      <c r="F4" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="35"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D4:D5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix the seventh test case and add an eight
</commit_message>
<xml_diff>
--- a/test/Test cases.xlsx
+++ b/test/Test cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\maze-project-2021\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6961E56-CD71-4CC4-8477-6734698380DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B29716-2664-40AA-B336-7D02CF42901C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27210" windowHeight="15990" activeTab="5" xr2:uid="{D88C0871-9CFF-47EC-A37B-1CA9AB3CB744}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27210" windowHeight="15990" activeTab="6" xr2:uid="{D88C0871-9CFF-47EC-A37B-1CA9AB3CB744}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Лист4" sheetId="4" r:id="rId4"/>
     <sheet name="Лист5" sheetId="5" r:id="rId5"/>
     <sheet name="Лист6" sheetId="6" r:id="rId6"/>
+    <sheet name="Лист7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -139,16 +140,20 @@
     <t>2.Check the weather the "if" condition statements in the function work</t>
   </si>
   <si>
-    <t>1.The function takes the with and height</t>
-  </si>
-  <si>
     <t>2. The "if" condition statements work and a result is received</t>
   </si>
   <si>
-    <t>1.The function successfully takes the with and height</t>
-  </si>
-  <si>
     <t>2.The "if" condition statements works and a the function returns "true" or "false"</t>
+  </si>
+  <si>
+    <t>Function 
+toIndex in maze</t>
+  </si>
+  <si>
+    <t>1.The function takes the inputed values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.The function successfully takes the inputed values </t>
   </si>
 </sst>
 </file>
@@ -417,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -531,6 +536,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Нормален" xfId="0" builtinId="0"/>
@@ -1583,8 +1592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDD3808-7269-4705-8859-387567E01703}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1631,13 +1640,13 @@
         <v>26</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G2" s="19" t="s">
         <v>13</v>
@@ -1659,11 +1668,11 @@
         <v>27</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="40"/>
       <c r="F4" s="36" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G4" s="35"/>
     </row>
@@ -1693,4 +1702,96 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0A2D3D-D73B-4F44-8C59-C739055D02A8}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
+        <v>8</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="41"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="41"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="41"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="42"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update the eighth testcase
</commit_message>
<xml_diff>
--- a/test/Test cases.xlsx
+++ b/test/Test cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\maze-project-2021\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B29716-2664-40AA-B336-7D02CF42901C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C8D858-736A-46CC-8BD0-C10A71845A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27210" windowHeight="15990" activeTab="6" xr2:uid="{D88C0871-9CFF-47EC-A37B-1CA9AB3CB744}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="38">
   <si>
     <t>ID</t>
   </si>
@@ -154,6 +154,21 @@
   </si>
   <si>
     <t xml:space="preserve">1.The function successfully takes the inputed values </t>
+  </si>
+  <si>
+    <t>1.Check if the function takes all needed inputs</t>
+  </si>
+  <si>
+    <t>2.Check if the function calculates everything right and returns a result</t>
+  </si>
+  <si>
+    <t>1.Function successfully takes all input</t>
+  </si>
+  <si>
+    <t>2.The function calculates and returns a result</t>
+  </si>
+  <si>
+    <t>1.Function takes the given inputs</t>
   </si>
 </sst>
 </file>
@@ -422,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -536,10 +551,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Нормален" xfId="0" builtinId="0"/>
@@ -1709,7 +1726,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,51 +1762,75 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="33.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21">
         <v>8</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="41"/>
+      <c r="C2" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="35"/>
       <c r="B3" s="35"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="41"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" s="42"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="35"/>
+    </row>
+    <row r="4" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="35"/>
       <c r="B4" s="35"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="41"/>
+      <c r="C4" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="40"/>
+      <c r="F4" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="35"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22"/>
       <c r="B5" s="22"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="42"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="10">
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G2:G5"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D4:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>